<commit_message>
fix em varias coisas
fixado bug no nome das quests
fixado bug na descricao das quests
fixado bug  em caminhos longos

parece queo bug era nos arquivos do jogo, mas com isso, fiz um "remendo"
</commit_message>
<xml_diff>
--- a/PTBR/Lang/PTBR/Dialog/Drama/_chara.xlsx
+++ b/PTBR/Lang/PTBR/Dialog/Drama/_chara.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isy\Documents\GitHub\elin-portugues-brasileiro\Traduzido\PTBR\Lang\PTBR\Dialog\Drama\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Elin\Package\PTBR\Lang\PTBR\Dialog\Drama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8736BD9-D365-4CEF-B9ED-0B4BCCD9132C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274DAE68-E0AF-4650-8757-4C8637C8313A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -329,9 +329,6 @@
     <t>Junte-se a nós! #1</t>
   </si>
   <si>
-    <t>Por favor, vá embora.</t>
-  </si>
-  <si>
     <t>Eu chamarei #1 agora.</t>
   </si>
   <si>
@@ -344,9 +341,6 @@
     <t>Me leve em segurança até meu destino.</t>
   </si>
   <si>
-    <t>Me dê #1, ou sua vida estará perdida!</t>
-  </si>
-  <si>
     <t>Eu me rendo. (Perde: #2)</t>
   </si>
   <si>
@@ -375,6 +369,12 @@
   </si>
   <si>
     <t>É uma decisão bastante sábia.</t>
+  </si>
+  <si>
+    <t>Mudei de ideia.</t>
+  </si>
+  <si>
+    <t>Se valoriza sua vida, entregue #1 sem resistência!</t>
   </si>
 </sst>
 </file>
@@ -638,9 +638,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K123" sqref="K123"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K109" sqref="K109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -939,7 +939,7 @@
         <v>40</v>
       </c>
       <c r="K41" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -1039,7 +1039,7 @@
         <v>49</v>
       </c>
       <c r="K61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -1071,7 +1071,7 @@
         <v>54</v>
       </c>
       <c r="K66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -1095,7 +1095,7 @@
         <v>57</v>
       </c>
       <c r="K70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -1119,7 +1119,7 @@
         <v>60</v>
       </c>
       <c r="K74" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -1143,7 +1143,7 @@
         <v>63</v>
       </c>
       <c r="K79" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -1157,7 +1157,7 @@
         <v>65</v>
       </c>
       <c r="K80" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:11">
@@ -1186,7 +1186,7 @@
         <v>68</v>
       </c>
       <c r="K85" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="86" spans="1:11">
@@ -1215,7 +1215,7 @@
         <v>71</v>
       </c>
       <c r="K91" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:11">
@@ -1239,7 +1239,7 @@
         <v>74</v>
       </c>
       <c r="K95" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="96" spans="1:11">
@@ -1263,7 +1263,7 @@
         <v>77</v>
       </c>
       <c r="K100" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:11">
@@ -1287,7 +1287,7 @@
         <v>80</v>
       </c>
       <c r="K104" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="105" spans="1:11">
@@ -1311,7 +1311,7 @@
         <v>83</v>
       </c>
       <c r="K109" s="4" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
     </row>
     <row r="110" spans="1:11">
@@ -1335,7 +1335,7 @@
         <v>86</v>
       </c>
       <c r="K111" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:11">
@@ -1355,7 +1355,7 @@
         <v>89</v>
       </c>
       <c r="K112" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="113" spans="1:11">
@@ -1401,7 +1401,7 @@
         <v>92</v>
       </c>
       <c r="K123" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="124" spans="1:11">

</xml_diff>